<commit_message>
Acrescentado informações sobre "apenpyxl".
</commit_message>
<xml_diff>
--- a/Secao 5 - Módulos Python/Aula.150 Openpyxl - Planilhas do Excel/nova_planilha.xlsx
+++ b/Secao 5 - Módulos Python/Aula.150 Openpyxl - Planilhas do Excel/nova_planilha.xlsx
@@ -436,7 +436,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>R$ 87.36</t>
+          <t>R$ 18.72</t>
         </is>
       </c>
     </row>
@@ -453,7 +453,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 26.99</t>
+          <t>R$ 72.22</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 84.31</t>
+          <t>R$ 28.34</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>R$ 54.12</t>
+          <t>R$ 21.57</t>
         </is>
       </c>
     </row>
@@ -504,7 +504,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 17.21</t>
+          <t>R$ 20.91</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 85.27</t>
+          <t>R$ 61.49</t>
         </is>
       </c>
     </row>
@@ -538,7 +538,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 10.48</t>
+          <t>R$ 71.72</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 84.0</t>
+          <t>R$ 36.96</t>
         </is>
       </c>
     </row>
@@ -572,7 +572,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 98.67</t>
+          <t>R$ 76.9</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 55.65</t>
+          <t>R$ 66.75</t>
         </is>
       </c>
     </row>
@@ -615,220 +615,220 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>cód 75</t>
+          <t>cód 94</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>R$ 88.61</t>
+          <t>R$ 93.66</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>R$ 67.85</t>
+          <t>R$ 18.12</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>R$ 98.61</t>
+          <t>R$ 80.4</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cód 49</t>
+          <t>cód 66</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 87.18</t>
+          <t>R$ 95.56</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 68.04</t>
+          <t>R$ 84.4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 94.15</t>
+          <t>R$ 55.68</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cód 68</t>
+          <t>cód 87</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 87.34</t>
+          <t>R$ 85.3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 54.26</t>
+          <t>R$ 33.41</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 41.74</t>
+          <t>R$ 47.3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cód 102</t>
+          <t>cód 34</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 81.38</t>
+          <t>R$ 89.22</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>R$ 57.48</t>
+          <t>R$ 67.24</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 72.78</t>
+          <t>R$ 14.08</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cód 90</t>
+          <t>cód 39</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 14.83</t>
+          <t>R$ 44.44</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 28.06</t>
+          <t>R$ 14.25</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 76.46</t>
+          <t>R$ 24.62</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>cód 42</t>
+          <t>cód 81</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 88.64</t>
+          <t>R$ 21.12</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 59.18</t>
+          <t>R$ 82.64</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 22.4</t>
+          <t>R$ 90.49</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cód 53</t>
+          <t>cód 49</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 26.62</t>
+          <t>R$ 49.6</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 44.5</t>
+          <t>R$ 86.09</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 47.13</t>
+          <t>R$ 23.6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>cód 56</t>
+          <t>cód 79</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 23.73</t>
+          <t>R$ 63.48</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 52.7</t>
+          <t>R$ 98.14</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 44.81</t>
+          <t>R$ 45.39</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cód 99</t>
+          <t>cód 57</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 28.42</t>
+          <t>R$ 70.49</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 28.18</t>
+          <t>R$ 41.72</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 49.13</t>
+          <t>R$ 29.94</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>cód 87</t>
+          <t>cód 64</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 97.07</t>
+          <t>R$ 88.22</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 36.8</t>
+          <t>R$ 60.62</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 26.31</t>
+          <t>R$ 55.42</t>
         </is>
       </c>
     </row>

</xml_diff>